<commit_message>
Agregada opción de eliminar clientes y actualizar HTML
</commit_message>
<xml_diff>
--- a/uploads/clientes.xlsx
+++ b/uploads/clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1395,36 +1395,6 @@
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>MIRTHA DELGADO</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>10.21.21.170/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>MARCELA LOOR</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>10.22.22.10/32</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>